<commit_message>
modified:   Readme.md 	modified:   Windsor-20250922.xlsx 	new file:   pairings.json 	new file:   protein copy.ipynb 	modified:   protein.ipynb 	modified:   protein.py
</commit_message>
<xml_diff>
--- a/Windsor-20250922.xlsx
+++ b/Windsor-20250922.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yutik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yutik\Downloads\TheProteinCult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D6F2218-D296-4DA8-B571-7EE28932C17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B988A5-21FE-4508-9AEF-0F69292B3599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{ADFCAE73-49BC-4407-B3DF-97E0C34A612D}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{ADFCAE73-49BC-4407-B3DF-97E0C34A612D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>Food Items</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>1/3 cup</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
   <si>
     <t>1 each</t>
@@ -580,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6A9427-0657-4EF6-9D58-E591A1A64027}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>82</v>
@@ -733,7 +730,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>202</v>
@@ -748,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -756,7 +753,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <v>221</v>
@@ -779,7 +776,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9">
         <v>120</v>
@@ -802,7 +799,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>51</v>
@@ -825,7 +822,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11">
         <v>103</v>
@@ -848,7 +845,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>140</v>
@@ -871,7 +868,7 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>152</v>
@@ -886,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -894,7 +891,7 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <v>74</v>
@@ -917,7 +914,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15">
         <v>372</v>
@@ -932,7 +929,7 @@
         <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -940,7 +937,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>50</v>
@@ -963,7 +960,7 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -986,7 +983,7 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1009,7 +1006,7 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19">
         <v>31</v>
@@ -1032,7 +1029,7 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20">
         <v>4</v>
@@ -1055,7 +1052,7 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21">
         <v>94</v>
@@ -1078,7 +1075,7 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -1101,7 +1098,7 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23">
         <v>160</v>
@@ -1124,7 +1121,7 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24">
         <v>96</v>
@@ -1147,7 +1144,7 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25">
         <v>249</v>
@@ -1170,7 +1167,7 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26">
         <v>70</v>
@@ -1193,7 +1190,7 @@
         <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27">
         <v>80</v>
@@ -1216,7 +1213,7 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28">
         <v>18</v>
@@ -1239,7 +1236,7 @@
         <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29">
         <v>100</v>
@@ -1262,7 +1259,7 @@
         <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30">
         <v>214</v>
@@ -1285,7 +1282,7 @@
         <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31">
         <v>361</v>
@@ -1308,7 +1305,7 @@
         <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32">
         <v>111</v>
@@ -1354,7 +1351,7 @@
         <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34">
         <v>271</v>

</xml_diff>